<commit_message>
Updating the overall plot and table (overall results)
</commit_message>
<xml_diff>
--- a/data/Table results.xlsx
+++ b/data/Table results.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamanw\Dropbox\Meta Analysis Project\Extraction\Transgenerational Meta-Analysis\R\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Dropbox\Meta Analysis Project\Extraction\Transgenerational Meta-Analysis\R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7203B49-B690-4C54-A013-1BDE7F11015E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FB3181-3585-4C59-A878-8059E2446EF2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7CE0AC1-5B38-41F4-A05C-6CFBC39CF1AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{B7CE0AC1-5B38-41F4-A05C-6CFBC39CF1AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
   <si>
     <t>ci.lb</t>
   </si>
@@ -451,7 +450,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,8 +600,7 @@
         <v>0.30249999999999999</v>
       </c>
       <c r="D5">
-        <f>0.0521-0.7377</f>
-        <v>-0.68559999999999999</v>
+        <v>-0.73770000000000002</v>
       </c>
       <c r="E5">
         <v>0.50800000000000001</v>

</xml_diff>

<commit_message>
Updating the code to make it look cleaner and start devloping plots for overall analysis for lnRR
</commit_message>
<xml_diff>
--- a/data/Table results.xlsx
+++ b/data/Table results.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Dropbox\Meta Analysis Project\Extraction\Transgenerational Meta-Analysis\R\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamanw\Dropbox\Meta Analysis Project\Extraction\Transgenerational Meta-Analysis\R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FB3181-3585-4C59-A878-8059E2446EF2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A34217B-C2B9-44A6-A338-C036D77CD8F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{B7CE0AC1-5B38-41F4-A05C-6CFBC39CF1AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7CE0AC1-5B38-41F4-A05C-6CFBC39CF1AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
   <si>
     <t>ci.lb</t>
   </si>
@@ -39,9 +40,6 @@
   </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>Overall</t>
   </si>
   <si>
     <t>MG</t>
@@ -102,13 +100,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,8 +134,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,28 +453,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25618584-ABCA-4AD8-9FEF-A38FDD27F1E1}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C12" sqref="C12:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -477,39 +483,39 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>0.4002</v>
+        <v>0.4173</v>
       </c>
       <c r="D2">
-        <v>5.4300000000000001E-2</v>
+        <v>5.21E-2</v>
       </c>
       <c r="E2">
-        <v>0.746</v>
+        <v>0.78259999999999996</v>
       </c>
       <c r="F2">
-        <v>2.3300000000000001E-2</v>
+        <v>2.5100000000000001E-2</v>
       </c>
       <c r="G2">
         <v>118</v>
@@ -526,31 +532,31 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>7.1099999999999997E-2</v>
+        <v>11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-0.1148</v>
       </c>
       <c r="D3">
-        <v>2.23E-2</v>
+        <v>-0.73770000000000002</v>
       </c>
       <c r="E3">
-        <v>0.12</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="F3">
-        <v>4.3E-3</v>
+        <v>0.71779999999999999</v>
       </c>
       <c r="G3">
-        <v>223</v>
+        <v>118</v>
       </c>
       <c r="H3">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I3">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="J3">
         <v>6</v>
@@ -561,28 +567,28 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>0.4173</v>
+        <v>0.18729999999999999</v>
       </c>
       <c r="D4">
-        <v>5.21E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="E4">
-        <v>0.78259999999999996</v>
-      </c>
-      <c r="F4">
-        <v>2.5100000000000001E-2</v>
+        <v>0.28160000000000002</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
       </c>
       <c r="G4">
-        <v>118</v>
+        <v>223</v>
       </c>
       <c r="H4">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I4">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="J4">
         <v>6</v>
@@ -593,29 +599,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <f>0.4173-0.1148</f>
-        <v>0.30249999999999999</v>
+        <v>-0.11260000000000001</v>
       </c>
       <c r="D5">
-        <v>-0.73770000000000002</v>
+        <v>-0.19869999999999999</v>
       </c>
       <c r="E5">
-        <v>0.50800000000000001</v>
+        <v>-2.6499999999999999E-2</v>
       </c>
       <c r="F5">
-        <v>0.71779999999999999</v>
+        <v>1.04E-2</v>
       </c>
       <c r="G5">
-        <v>118</v>
+        <v>223</v>
       </c>
       <c r="H5">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I5">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="J5">
         <v>6</v>
@@ -623,22 +628,22 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>0.18729999999999999</v>
+        <v>-0.13819999999999999</v>
       </c>
       <c r="D6">
-        <v>9.2999999999999999E-2</v>
+        <v>-0.21920000000000001</v>
       </c>
       <c r="E6">
-        <v>0.28160000000000002</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
+        <v>-5.7099999999999998E-2</v>
+      </c>
+      <c r="F6">
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="G6">
         <v>223</v>
@@ -655,32 +660,31 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <f>0.1873-0.1126</f>
-        <v>7.4699999999999989E-2</v>
+        <v>0.44419999999999998</v>
       </c>
       <c r="D7">
-        <v>-0.19869999999999999</v>
+        <v>4.9599999999999998E-2</v>
       </c>
       <c r="E7">
-        <v>-2.6499999999999999E-2</v>
+        <v>0.83879999999999999</v>
       </c>
       <c r="F7">
-        <v>1.04E-2</v>
+        <v>2.7400000000000001E-2</v>
       </c>
       <c r="G7">
-        <v>223</v>
+        <v>118</v>
       </c>
       <c r="H7">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I7">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="J7">
         <v>6</v>
@@ -688,32 +692,31 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <f>0.1873-0.1382</f>
-        <v>4.9100000000000005E-2</v>
+        <v>-0.11409999999999999</v>
       </c>
       <c r="D8">
-        <v>-0.21920000000000001</v>
+        <v>-0.5756</v>
       </c>
       <c r="E8">
-        <v>-5.7099999999999998E-2</v>
+        <v>0.34739999999999999</v>
       </c>
       <c r="F8">
-        <v>8.0000000000000004E-4</v>
+        <v>0.628</v>
       </c>
       <c r="G8">
-        <v>223</v>
+        <v>118</v>
       </c>
       <c r="H8">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I8">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="J8">
         <v>6</v>
@@ -724,28 +727,28 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>0.44419999999999998</v>
+        <v>7.4300000000000005E-2</v>
       </c>
       <c r="D9">
-        <v>4.9599999999999998E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="E9">
-        <v>0.83879999999999999</v>
+        <v>0.12609999999999999</v>
       </c>
       <c r="F9">
-        <v>2.7400000000000001E-2</v>
+        <v>4.8999999999999998E-3</v>
       </c>
       <c r="G9">
-        <v>118</v>
+        <v>223</v>
       </c>
       <c r="H9">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I9">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="J9">
         <v>6</v>
@@ -756,29 +759,28 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="D10">
+        <v>-7.2099999999999997E-2</v>
+      </c>
+      <c r="E10">
+        <v>4.82E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.69640000000000002</v>
+      </c>
+      <c r="G10">
+        <v>223</v>
+      </c>
+      <c r="H10">
         <v>16</v>
       </c>
-      <c r="C10">
-        <f>0.4442-0.1141</f>
-        <v>0.3301</v>
-      </c>
-      <c r="D10">
-        <v>-0.5756</v>
-      </c>
-      <c r="E10">
-        <v>0.34739999999999999</v>
-      </c>
-      <c r="F10">
-        <v>0.628</v>
-      </c>
-      <c r="G10">
-        <v>118</v>
-      </c>
-      <c r="H10">
-        <v>13</v>
-      </c>
       <c r="I10">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="J10">
         <v>6</v>
@@ -786,31 +788,31 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>7.4300000000000005E-2</v>
+        <v>1.0519000000000001</v>
       </c>
       <c r="D11">
-        <v>2.2599999999999999E-2</v>
+        <v>0.48420000000000002</v>
       </c>
       <c r="E11">
-        <v>0.12609999999999999</v>
+        <v>1.6195999999999999</v>
       </c>
       <c r="F11">
-        <v>4.8999999999999998E-3</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="G11">
-        <v>223</v>
+        <v>118</v>
       </c>
       <c r="H11">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I11">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="J11">
         <v>6</v>
@@ -818,32 +820,31 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12">
-        <f>0.0743-0.012</f>
-        <v>6.2300000000000008E-2</v>
+        <v>-0.93479999999999996</v>
       </c>
       <c r="D12">
-        <v>-7.2099999999999997E-2</v>
+        <v>-1.3164</v>
       </c>
       <c r="E12">
-        <v>4.82E-2</v>
-      </c>
-      <c r="F12">
-        <v>0.69640000000000002</v>
+        <v>-0.55310000000000004</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
       </c>
       <c r="G12">
-        <v>223</v>
+        <v>118</v>
       </c>
       <c r="H12">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I12">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="J12">
         <v>6</v>
@@ -851,22 +852,22 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13">
-        <v>1.0519000000000001</v>
+        <v>-0.92730000000000001</v>
       </c>
       <c r="D13">
-        <v>0.48420000000000002</v>
+        <v>-1.3147</v>
       </c>
       <c r="E13">
-        <v>1.6195999999999999</v>
-      </c>
-      <c r="F13">
-        <v>2.9999999999999997E-4</v>
+        <v>-0.53990000000000005</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
       </c>
       <c r="G13">
         <v>118</v>
@@ -886,29 +887,28 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14">
-        <f>1.0519-0.9348</f>
-        <v>0.11710000000000009</v>
+        <v>-0.38019999999999998</v>
       </c>
       <c r="D14">
-        <v>-1.3164</v>
+        <v>-0.65359999999999996</v>
       </c>
       <c r="E14">
-        <v>-0.55310000000000004</v>
-      </c>
-      <c r="F14" t="s">
-        <v>14</v>
+        <v>-0.10680000000000001</v>
+      </c>
+      <c r="F14">
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="G14">
-        <v>118</v>
+        <v>223</v>
       </c>
       <c r="H14">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I14">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="J14">
         <v>6</v>
@@ -919,29 +919,28 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15">
-        <f>1.0519-0.9273</f>
-        <v>0.12460000000000004</v>
+        <v>0.45300000000000001</v>
       </c>
       <c r="D15">
-        <v>-1.3147</v>
+        <v>0.18</v>
       </c>
       <c r="E15">
-        <v>-0.53990000000000005</v>
-      </c>
-      <c r="F15" t="s">
-        <v>14</v>
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="F15">
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="G15">
-        <v>118</v>
+        <v>223</v>
       </c>
       <c r="H15">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I15">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="J15">
         <v>6</v>
@@ -949,22 +948,22 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16">
-        <v>-0.38019999999999998</v>
+        <v>0.45910000000000001</v>
       </c>
       <c r="D16">
-        <v>-0.65359999999999996</v>
+        <v>0.18629999999999999</v>
       </c>
       <c r="E16">
-        <v>-0.10680000000000001</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="F16">
-        <v>6.4000000000000003E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="G16">
         <v>223</v>
@@ -979,73 +978,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17">
-        <f>-0.3802+0.453</f>
-        <v>7.2800000000000031E-2</v>
-      </c>
-      <c r="D17">
-        <v>0.18</v>
-      </c>
-      <c r="E17">
-        <v>0.72599999999999998</v>
-      </c>
-      <c r="F17">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="G17">
-        <v>223</v>
-      </c>
-      <c r="H17">
-        <v>16</v>
-      </c>
-      <c r="I17">
-        <v>52</v>
-      </c>
-      <c r="J17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18">
-        <f>-0.3802+0.4591</f>
-        <v>7.8900000000000026E-2</v>
-      </c>
-      <c r="D18">
-        <v>0.18629999999999999</v>
-      </c>
-      <c r="E18">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="F18">
-        <v>1E-3</v>
-      </c>
-      <c r="G18">
-        <v>223</v>
-      </c>
-      <c r="H18">
-        <v>16</v>
-      </c>
-      <c r="I18">
-        <v>52</v>
-      </c>
-      <c r="J18">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created another RMD file to show the results. I need to clean up the other files and organize correctly
</commit_message>
<xml_diff>
--- a/data/Table results.xlsx
+++ b/data/Table results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamanw\Dropbox\Meta Analysis Project\Extraction\Transgenerational Meta-Analysis\R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A34217B-C2B9-44A6-A338-C036D77CD8F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F48443D-EB33-4961-8588-ABBC72EF7637}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7CE0AC1-5B38-41F4-A05C-6CFBC39CF1AA}"/>
   </bookViews>
@@ -63,15 +63,6 @@
     <t>traits</t>
   </si>
   <si>
-    <t>Female_F0</t>
-  </si>
-  <si>
-    <t>Male_F0</t>
-  </si>
-  <si>
-    <t>Both_F0</t>
-  </si>
-  <si>
     <t>&lt;0.0001</t>
   </si>
   <si>
@@ -81,9 +72,6 @@
     <t>Rat</t>
   </si>
   <si>
-    <t>Both_Sex Grand Offspring</t>
-  </si>
-  <si>
     <t>Female Grand Offspring</t>
   </si>
   <si>
@@ -94,6 +82,18 @@
   </si>
   <si>
     <t>Effect_Size_lnRR</t>
+  </si>
+  <si>
+    <t>Female F0</t>
+  </si>
+  <si>
+    <t>Male F0</t>
+  </si>
+  <si>
+    <t>Both F0</t>
+  </si>
+  <si>
+    <t>Grand Offspring (Both Sex)</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,13 +468,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -503,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>0.4173</v>
@@ -535,7 +535,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1">
         <v>-0.1148</v>
@@ -567,7 +567,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>0.18729999999999999</v>
@@ -579,7 +579,7 @@
         <v>0.28160000000000002</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>223</v>
@@ -599,7 +599,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>-0.11260000000000001</v>
@@ -631,7 +631,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>-0.13819999999999999</v>
@@ -663,7 +663,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>0.44419999999999998</v>
@@ -695,7 +695,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>-0.11409999999999999</v>
@@ -727,7 +727,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>7.4300000000000005E-2</v>
@@ -759,7 +759,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>-1.2E-2</v>
@@ -791,7 +791,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>1.0519000000000001</v>
@@ -823,7 +823,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>-0.93479999999999996</v>
@@ -835,7 +835,7 @@
         <v>-0.55310000000000004</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G12">
         <v>118</v>
@@ -855,7 +855,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>-0.92730000000000001</v>
@@ -867,7 +867,7 @@
         <v>-0.53990000000000005</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G13">
         <v>118</v>
@@ -887,7 +887,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <v>-0.38019999999999998</v>
@@ -919,7 +919,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>0.45300000000000001</v>
@@ -951,7 +951,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>0.45910000000000001</v>

</xml_diff>